<commit_message>
fixed data management error in employment, removed decline to answer from health literacy variables, and assigment 3 vizzes
</commit_message>
<xml_diff>
--- a/all managed data.xlsx
+++ b/all managed data.xlsx
@@ -642,6 +642,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L5" t="inlineStr">
         <is>
           <t>Occasionally</t>
@@ -705,6 +710,11 @@
           <t>In Poverty</t>
         </is>
       </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L6" t="inlineStr">
         <is>
           <t>Never</t>
@@ -2271,6 +2281,11 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L31" t="inlineStr">
         <is>
           <t>Occasionally</t>
@@ -2558,6 +2573,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L35" t="inlineStr">
         <is>
           <t>Never</t>
@@ -3426,6 +3446,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K48" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L48" t="inlineStr">
         <is>
           <t>Occasionally</t>
@@ -5914,6 +5939,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K85" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L85" t="inlineStr">
         <is>
           <t>Never</t>
@@ -6055,6 +6085,11 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="K87" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L87" t="inlineStr">
         <is>
           <t>Never</t>
@@ -6123,6 +6158,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K88" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L88" t="inlineStr">
         <is>
           <t>Often</t>
@@ -6546,6 +6586,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K94" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L94" t="inlineStr">
         <is>
           <t>Never</t>
@@ -7646,6 +7691,11 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="K110" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L110" t="inlineStr">
         <is>
           <t>Occasionally</t>
@@ -8142,6 +8192,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K117" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L117" t="inlineStr">
         <is>
           <t>Never</t>
@@ -8581,6 +8636,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K125" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L125" t="inlineStr">
         <is>
           <t>Sometimes</t>
@@ -9517,6 +9577,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K138" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L138" t="inlineStr">
         <is>
           <t>Often</t>
@@ -9804,6 +9869,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K142" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L142" t="inlineStr">
         <is>
           <t>Occasionally</t>
@@ -13407,6 +13477,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K196" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L196" t="inlineStr">
         <is>
           <t>Sometimes</t>
@@ -13606,6 +13681,11 @@
           <t>Not in Poverty</t>
         </is>
       </c>
+      <c r="K199" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L199" t="inlineStr">
         <is>
           <t>Always</t>
@@ -13810,6 +13890,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K202" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L202" t="inlineStr">
         <is>
           <t>Never</t>
@@ -13878,6 +13963,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K203" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L203" t="inlineStr">
         <is>
           <t>Sometimes</t>
@@ -14228,6 +14318,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K208" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L208" t="inlineStr">
         <is>
           <t>Always</t>
@@ -14719,6 +14814,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K215" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L215" t="inlineStr">
         <is>
           <t>Sometimes</t>
@@ -14933,6 +15033,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K218" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L218" t="inlineStr">
         <is>
           <t>Always</t>
@@ -15711,6 +15816,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K229" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L229" t="inlineStr">
         <is>
           <t>Never</t>
@@ -15779,6 +15889,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K230" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L230" t="inlineStr">
         <is>
           <t>Always</t>
@@ -15917,6 +16032,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K232" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L232" t="inlineStr">
         <is>
           <t>Never</t>
@@ -16559,6 +16679,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K241" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L241" t="inlineStr">
         <is>
           <t>Occasionally</t>
@@ -16768,6 +16893,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K244" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L244" t="inlineStr">
         <is>
           <t>Sometimes</t>
@@ -16904,6 +17034,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K246" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L246" t="inlineStr">
         <is>
           <t>Never</t>
@@ -17410,6 +17545,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K253" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L253" t="inlineStr">
         <is>
           <t>Never</t>
@@ -18047,6 +18187,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K262" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L262" t="inlineStr">
         <is>
           <t>Never</t>
@@ -18654,6 +18799,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K271" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L271" t="inlineStr">
         <is>
           <t>Occasionally</t>
@@ -18795,6 +18945,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K273" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L273" t="inlineStr">
         <is>
           <t>Sometimes</t>
@@ -21003,6 +21158,11 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="K304" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L304" t="inlineStr">
         <is>
           <t>Never</t>
@@ -21494,6 +21654,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K311" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L311" t="inlineStr">
         <is>
           <t>Sometimes</t>
@@ -21841,6 +22006,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K316" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L316" t="inlineStr">
         <is>
           <t>Never</t>
@@ -22201,6 +22371,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K321" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L321" t="inlineStr">
         <is>
           <t>Sometimes</t>
@@ -22561,6 +22736,11 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="K326" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L326" t="inlineStr">
         <is>
           <t>Occasionally</t>
@@ -22843,6 +23023,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K330" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L330" t="inlineStr">
         <is>
           <t>Sometimes</t>
@@ -22911,6 +23096,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K331" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L331" t="inlineStr">
         <is>
           <t>Always</t>
@@ -22979,6 +23169,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K332" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L332" t="inlineStr">
         <is>
           <t>Never</t>
@@ -23110,6 +23305,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K334" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L334" t="inlineStr">
         <is>
           <t>Always</t>
@@ -23251,6 +23451,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K336" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L336" t="inlineStr">
         <is>
           <t>Sometimes</t>
@@ -23319,6 +23524,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K337" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L337" t="inlineStr">
         <is>
           <t>Always</t>
@@ -23387,6 +23597,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K338" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L338" t="inlineStr">
         <is>
           <t>Always</t>
@@ -23523,6 +23738,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K340" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L340" t="inlineStr">
         <is>
           <t>Always</t>
@@ -23744,6 +23964,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K344" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L344" t="inlineStr">
         <is>
           <t>Never</t>
@@ -23953,6 +24178,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K347" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L347" t="inlineStr">
         <is>
           <t>Sometimes</t>
@@ -24527,6 +24757,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K356" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L356" t="inlineStr">
         <is>
           <t>Never</t>
@@ -24595,6 +24830,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K357" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L357" t="inlineStr">
         <is>
           <t>Always</t>
@@ -24877,6 +25117,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K361" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L361" t="inlineStr">
         <is>
           <t>Sometimes</t>
@@ -25018,6 +25263,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K363" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L363" t="inlineStr">
         <is>
           <t>Never</t>
@@ -25284,6 +25534,11 @@
           <t>Not in Poverty</t>
         </is>
       </c>
+      <c r="K369" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L369" t="inlineStr">
         <is>
           <t>Sometimes</t>
@@ -25425,6 +25680,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K371" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L371" t="inlineStr">
         <is>
           <t>Always</t>
@@ -25669,6 +25929,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K376" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L376" t="inlineStr">
         <is>
           <t>Always</t>
@@ -25737,6 +26002,11 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="K377" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L377" t="inlineStr">
         <is>
           <t>Never</t>
@@ -25805,6 +26075,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K378" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L378" t="inlineStr">
         <is>
           <t>Occasionally</t>
@@ -25936,6 +26211,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K380" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L380" t="inlineStr">
         <is>
           <t>Always</t>
@@ -26092,6 +26372,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K383" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L383" t="inlineStr">
         <is>
           <t>Sometimes</t>
@@ -26306,6 +26591,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K386" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L386" t="inlineStr">
         <is>
           <t>Always</t>
@@ -27230,6 +27520,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K399" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L399" t="inlineStr">
         <is>
           <t>Never</t>
@@ -27298,6 +27593,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K400" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L400" t="inlineStr">
         <is>
           <t>Sometimes</t>
@@ -27429,6 +27729,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K402" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L402" t="inlineStr">
         <is>
           <t>Always</t>
@@ -27497,6 +27802,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K403" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L403" t="inlineStr">
         <is>
           <t>Always</t>
@@ -27565,6 +27875,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K404" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L404" t="inlineStr">
         <is>
           <t>Decline to answer</t>
@@ -27706,6 +28021,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K406" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L406" t="inlineStr">
         <is>
           <t>Always</t>
@@ -27920,6 +28240,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K409" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L409" t="inlineStr">
         <is>
           <t>Always</t>
@@ -28056,6 +28381,11 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="K411" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L411" t="inlineStr">
         <is>
           <t>Always</t>
@@ -28124,6 +28454,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K412" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L412" t="inlineStr">
         <is>
           <t>Sometimes</t>
@@ -28260,6 +28595,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K414" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L414" t="inlineStr">
         <is>
           <t>Often</t>
@@ -28328,6 +28668,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K415" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L415" t="inlineStr">
         <is>
           <t>Often</t>
@@ -28610,6 +28955,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K419" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L419" t="inlineStr">
         <is>
           <t>Always</t>
@@ -28678,6 +29028,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K420" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L420" t="inlineStr">
         <is>
           <t>Always</t>
@@ -28977,6 +29332,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K425" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L425" t="inlineStr">
         <is>
           <t>Always</t>
@@ -29556,6 +29916,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K433" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L433" t="inlineStr">
         <is>
           <t>Sometimes</t>
@@ -29624,6 +29989,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K434" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L434" t="inlineStr">
         <is>
           <t>Never</t>
@@ -29692,6 +30062,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K435" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L435" t="inlineStr">
         <is>
           <t>Often</t>
@@ -29848,6 +30223,11 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="K438" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L438" t="inlineStr">
         <is>
           <t>Sometimes</t>
@@ -29916,6 +30296,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K439" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L439" t="inlineStr">
         <is>
           <t>Occasionally</t>
@@ -29984,6 +30369,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K440" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L440" t="inlineStr">
         <is>
           <t>Never</t>
@@ -30286,6 +30676,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K445" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L445" t="inlineStr">
         <is>
           <t>Sometimes</t>
@@ -30427,6 +30822,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K447" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L447" t="inlineStr">
         <is>
           <t>Often</t>
@@ -30671,6 +31071,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K452" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L452" t="inlineStr">
         <is>
           <t>Always</t>
@@ -30739,6 +31144,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K453" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L453" t="inlineStr">
         <is>
           <t>Always</t>
@@ -31245,6 +31655,11 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="K460" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L460" t="inlineStr">
         <is>
           <t>Always</t>
@@ -31459,6 +31874,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K463" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L463" t="inlineStr">
         <is>
           <t>Occasionally</t>
@@ -31600,6 +32020,11 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="K465" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L465" t="inlineStr">
         <is>
           <t>Never</t>
@@ -31736,6 +32161,11 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="K467" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L467" t="inlineStr">
         <is>
           <t>Always</t>
@@ -32038,6 +32468,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K472" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L472" t="inlineStr">
         <is>
           <t>Always</t>
@@ -32179,6 +32614,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K474" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L474" t="inlineStr">
         <is>
           <t>Sometimes</t>
@@ -32247,6 +32687,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K475" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L475" t="inlineStr">
         <is>
           <t>Always</t>
@@ -32431,6 +32876,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K478" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L478" t="inlineStr">
         <is>
           <t>Always</t>
@@ -32499,6 +32949,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K479" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L479" t="inlineStr">
         <is>
           <t>Never</t>
@@ -32640,6 +33095,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K481" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L481" t="inlineStr">
         <is>
           <t>Often</t>
@@ -33594,6 +34054,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K495" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L495" t="inlineStr">
         <is>
           <t>Never</t>
@@ -33969,6 +34434,11 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="K501" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L501" t="inlineStr">
         <is>
           <t>Never</t>
@@ -34037,6 +34507,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K502" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L502" t="inlineStr">
         <is>
           <t>Never</t>
@@ -34550,6 +35025,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K514" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L514" t="inlineStr">
         <is>
           <t>Sometimes</t>
@@ -34706,6 +35186,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K517" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L517" t="inlineStr">
         <is>
           <t>Never</t>
@@ -34774,6 +35259,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K518" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L518" t="inlineStr">
         <is>
           <t>Never</t>
@@ -34842,6 +35332,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K519" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L519" t="inlineStr">
         <is>
           <t>Always</t>
@@ -35275,6 +35770,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K525" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L525" t="inlineStr">
         <is>
           <t>Never</t>
@@ -35343,6 +35843,11 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="K526" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L526" t="inlineStr">
         <is>
           <t>Never</t>
@@ -35411,6 +35916,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K527" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L527" t="inlineStr">
         <is>
           <t>Sometimes</t>
@@ -35476,6 +35986,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K528" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L528" t="inlineStr">
         <is>
           <t>Never</t>
@@ -35544,6 +36059,11 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="K529" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L529" t="inlineStr">
         <is>
           <t>Never</t>
@@ -35685,6 +36205,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K531" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L531" t="inlineStr">
         <is>
           <t>Never</t>
@@ -36060,6 +36585,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K538" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L538" t="inlineStr">
         <is>
           <t>Sometimes</t>
@@ -36362,6 +36892,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K543" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L543" t="inlineStr">
         <is>
           <t>Always</t>
@@ -36868,6 +37403,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K550" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L550" t="inlineStr">
         <is>
           <t>Never</t>
@@ -37009,6 +37549,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K552" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L552" t="inlineStr">
         <is>
           <t>Always</t>
@@ -37384,6 +37929,11 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="K558" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L558" t="inlineStr">
         <is>
           <t>Sometimes</t>
@@ -37452,6 +38002,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K559" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L559" t="inlineStr">
         <is>
           <t>Never</t>
@@ -37729,6 +38284,11 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="K563" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L563" t="inlineStr">
         <is>
           <t>Never</t>
@@ -37870,6 +38430,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K565" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L565" t="inlineStr">
         <is>
           <t>Never</t>
@@ -37938,6 +38503,11 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="K566" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L566" t="inlineStr">
         <is>
           <t>Never</t>
@@ -38079,6 +38649,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K568" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L568" t="inlineStr">
         <is>
           <t>Never</t>
@@ -38683,6 +39258,11 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="K578" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L578" t="inlineStr">
         <is>
           <t>Never</t>
@@ -39116,6 +39696,11 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="K584" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L584" t="inlineStr">
         <is>
           <t>Never</t>
@@ -39330,6 +39915,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K587" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L587" t="inlineStr">
         <is>
           <t>Never</t>
@@ -39617,6 +40207,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K591" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L591" t="inlineStr">
         <is>
           <t>Never</t>
@@ -39758,6 +40353,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K593" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L593" t="inlineStr">
         <is>
           <t>Never</t>
@@ -40060,6 +40660,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K598" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L598" t="inlineStr">
         <is>
           <t>Always</t>
@@ -40143,6 +40748,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K600" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L600" t="inlineStr">
         <is>
           <t>Always</t>
@@ -40591,6 +41201,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K607" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L607" t="inlineStr">
         <is>
           <t>Sometimes</t>
@@ -40656,6 +41271,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K608" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L608" t="inlineStr">
         <is>
           <t>Never</t>
@@ -40943,6 +41563,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K612" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L612" t="inlineStr">
         <is>
           <t>Never</t>
@@ -41011,6 +41636,11 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="K613" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L613" t="inlineStr">
         <is>
           <t>Always</t>
@@ -41439,6 +42069,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K619" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L619" t="inlineStr">
         <is>
           <t>Occasionally</t>
@@ -41580,6 +42215,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K621" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L621" t="inlineStr">
         <is>
           <t>Sometimes</t>
@@ -42599,6 +43239,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K639" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L639" t="inlineStr">
         <is>
           <t>Never</t>
@@ -42667,6 +43312,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K640" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L640" t="inlineStr">
         <is>
           <t>Always</t>
@@ -43104,6 +43754,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K648" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L648" t="inlineStr">
         <is>
           <t>Never</t>
@@ -43172,6 +43827,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K649" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L649" t="inlineStr">
         <is>
           <t>Always</t>
@@ -43557,6 +44217,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K656" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L656" t="inlineStr">
         <is>
           <t>Sometimes</t>
@@ -43771,6 +44436,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K659" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L659" t="inlineStr">
         <is>
           <t>Never</t>
@@ -44053,6 +44723,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K663" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L663" t="inlineStr">
         <is>
           <t>Never</t>
@@ -44498,6 +45173,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K670" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L670" t="inlineStr">
         <is>
           <t>Always</t>
@@ -44782,6 +45462,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K674" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L674" t="inlineStr">
         <is>
           <t>Often</t>
@@ -44845,6 +45530,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K675" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L675" t="inlineStr">
         <is>
           <t>Always</t>
@@ -45119,6 +45809,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K679" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L679" t="inlineStr">
         <is>
           <t>Never</t>
@@ -45250,6 +45945,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K681" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L681" t="inlineStr">
         <is>
           <t>Never</t>
@@ -45532,6 +46232,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K685" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L685" t="inlineStr">
         <is>
           <t>Often</t>
@@ -45600,6 +46305,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K686" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L686" t="inlineStr">
         <is>
           <t>Always</t>
@@ -46267,6 +46977,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K697" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L697" t="inlineStr">
         <is>
           <t>Decline to answer</t>
@@ -47319,6 +48034,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K714" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L714" t="inlineStr">
         <is>
           <t>Sometimes</t>
@@ -48562,6 +49282,11 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="K732" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L732" t="inlineStr">
         <is>
           <t>Often</t>
@@ -48868,6 +49593,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K738" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L738" t="inlineStr">
         <is>
           <t>Sometimes</t>
@@ -49542,6 +50272,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K749" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L749" t="inlineStr">
         <is>
           <t>Never</t>
@@ -49683,6 +50418,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K751" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L751" t="inlineStr">
         <is>
           <t>Always</t>
@@ -49897,6 +50637,11 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="K754" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L754" t="inlineStr">
         <is>
           <t>Occasionally</t>
@@ -50795,6 +51540,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K768" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L768" t="inlineStr">
         <is>
           <t>Never</t>
@@ -50863,6 +51613,11 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="K769" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L769" t="inlineStr">
         <is>
           <t>Often</t>
@@ -51165,6 +51920,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K774" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L774" t="inlineStr">
         <is>
           <t>Occasionally</t>
@@ -51447,6 +52207,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K778" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L778" t="inlineStr">
         <is>
           <t>Never</t>
@@ -51515,6 +52280,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K779" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L779" t="inlineStr">
         <is>
           <t>Always</t>
@@ -51583,6 +52353,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K780" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L780" t="inlineStr">
         <is>
           <t>Never</t>
@@ -51651,6 +52426,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K781" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L781" t="inlineStr">
         <is>
           <t>Always</t>
@@ -52388,6 +53168,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K792" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L792" t="inlineStr">
         <is>
           <t>Never</t>
@@ -52682,6 +53467,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K797" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L797" t="inlineStr">
         <is>
           <t>Never</t>
@@ -52823,6 +53613,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K799" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L799" t="inlineStr">
         <is>
           <t>Often</t>
@@ -53183,6 +53978,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K804" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L804" t="inlineStr">
         <is>
           <t>Occasionally</t>
@@ -53482,6 +54282,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K809" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L809" t="inlineStr">
         <is>
           <t>Always</t>
@@ -54068,6 +54873,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K819" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L819" t="inlineStr">
         <is>
           <t>Occasionally</t>
@@ -54574,6 +55384,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K826" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L826" t="inlineStr">
         <is>
           <t>Sometimes</t>
@@ -54637,6 +55452,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K827" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L827" t="inlineStr">
         <is>
           <t>Never</t>
@@ -54911,6 +55731,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K831" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L831" t="inlineStr">
         <is>
           <t>Never</t>
@@ -54979,6 +55804,11 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="K832" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L832" t="inlineStr">
         <is>
           <t>Sometimes</t>
@@ -55427,6 +56257,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K839" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L839" t="inlineStr">
         <is>
           <t>Sometimes</t>
@@ -55797,6 +56632,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K845" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L845" t="inlineStr">
         <is>
           <t>Occasionally</t>
@@ -55865,6 +56705,11 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="K846" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L846" t="inlineStr">
         <is>
           <t>Always</t>
@@ -56079,6 +56924,11 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="K849" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L849" t="inlineStr">
         <is>
           <t>Never</t>
@@ -56288,6 +57138,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K852" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L852" t="inlineStr">
         <is>
           <t>Never</t>
@@ -56429,6 +57284,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K854" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L854" t="inlineStr">
         <is>
           <t>Always</t>
@@ -56743,6 +57603,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K860" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L860" t="inlineStr">
         <is>
           <t>Always</t>
@@ -56884,6 +57749,11 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="K862" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L862" t="inlineStr">
         <is>
           <t>Never</t>
@@ -57105,6 +57975,11 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="K866" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L866" t="inlineStr">
         <is>
           <t>Always</t>
@@ -57319,6 +58194,11 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="K869" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L869" t="inlineStr">
         <is>
           <t>Never</t>
@@ -57460,6 +58340,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K871" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L871" t="inlineStr">
         <is>
           <t>Often</t>
@@ -57593,6 +58478,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K873" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L873" t="inlineStr">
         <is>
           <t>Never</t>
@@ -57890,6 +58780,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K878" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L878" t="inlineStr">
         <is>
           <t>Often</t>
@@ -58171,6 +59066,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K882" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L882" t="inlineStr">
         <is>
           <t>Never</t>
@@ -58385,6 +59285,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K885" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L885" t="inlineStr">
         <is>
           <t>Always</t>
@@ -58468,6 +59373,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K887" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L887" t="inlineStr">
         <is>
           <t>Never</t>
@@ -58765,6 +59675,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K892" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L892" t="inlineStr">
         <is>
           <t>Often</t>
@@ -58921,6 +59836,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K895" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L895" t="inlineStr">
         <is>
           <t>Always</t>
@@ -59203,6 +60123,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K900" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L900" t="inlineStr">
         <is>
           <t>Sometimes</t>
@@ -60062,6 +60987,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K913" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L913" t="inlineStr">
         <is>
           <t>Sometimes</t>
@@ -60776,6 +61706,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K927" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L927" t="inlineStr">
         <is>
           <t>Never</t>
@@ -60990,6 +61925,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K930" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L930" t="inlineStr">
         <is>
           <t>Often</t>
@@ -61201,6 +62141,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K933" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L933" t="inlineStr">
         <is>
           <t>Never</t>
@@ -61412,6 +62357,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K936" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L936" t="inlineStr">
         <is>
           <t>Sometimes</t>
@@ -62466,6 +63416,11 @@
           <t>Not in Poverty</t>
         </is>
       </c>
+      <c r="K955" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L955" t="inlineStr">
         <is>
           <t>Decline to answer</t>
@@ -63366,6 +64321,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K970" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L970" t="inlineStr">
         <is>
           <t>Occasionally</t>
@@ -63580,6 +64540,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K973" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L973" t="inlineStr">
         <is>
           <t>Sometimes</t>
@@ -63711,6 +64676,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K975" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L975" t="inlineStr">
         <is>
           <t>Always</t>
@@ -63922,6 +64892,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K978" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L978" t="inlineStr">
         <is>
           <t>Sometimes</t>
@@ -64063,6 +65038,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K980" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L980" t="inlineStr">
         <is>
           <t>Decline to answer</t>
@@ -64126,6 +65106,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K981" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L981" t="inlineStr">
         <is>
           <t>Never</t>
@@ -64418,6 +65403,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K986" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L986" t="inlineStr">
         <is>
           <t>Never</t>
@@ -64486,6 +65476,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K987" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L987" t="inlineStr">
         <is>
           <t>Decline to answer</t>
@@ -64569,6 +65564,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K989" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L989" t="inlineStr">
         <is>
           <t>Often</t>
@@ -64637,6 +65637,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K990" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L990" t="inlineStr">
         <is>
           <t>Occasionally</t>
@@ -64778,6 +65783,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K992" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L992" t="inlineStr">
         <is>
           <t>Always</t>
@@ -64967,6 +65977,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K995" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L995" t="inlineStr">
         <is>
           <t>Occasionally</t>
@@ -65035,6 +66050,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K996" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L996" t="inlineStr">
         <is>
           <t>Always</t>
@@ -65571,6 +66591,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K1005" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L1005" t="inlineStr">
         <is>
           <t>Never</t>
@@ -65918,6 +66943,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K1010" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L1010" t="inlineStr">
         <is>
           <t>Often</t>
@@ -66200,6 +67230,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K1014" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L1014" t="inlineStr">
         <is>
           <t>Occasionally</t>
@@ -66268,6 +67303,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K1015" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L1015" t="inlineStr">
         <is>
           <t>Always</t>
@@ -67219,6 +68259,11 @@
           <t>Not in Poverty</t>
         </is>
       </c>
+      <c r="K1031" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L1031" t="inlineStr">
         <is>
           <t>Always</t>
@@ -67282,6 +68327,11 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="K1032" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L1032" t="inlineStr">
         <is>
           <t>Always</t>
@@ -67345,6 +68395,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K1033" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L1033" t="inlineStr">
         <is>
           <t>Always</t>
@@ -67410,6 +68465,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K1034" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L1034" t="inlineStr">
         <is>
           <t>Never</t>
@@ -68124,6 +69184,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K1045" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L1045" t="inlineStr">
         <is>
           <t>Never</t>
@@ -68192,6 +69257,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K1046" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L1046" t="inlineStr">
         <is>
           <t>Always</t>
@@ -69103,6 +70173,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K1063" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L1063" t="inlineStr">
         <is>
           <t>Decline to answer</t>
@@ -69171,6 +70246,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K1064" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L1064" t="inlineStr">
         <is>
           <t>Always</t>
@@ -69379,6 +70459,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K1067" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L1067" t="inlineStr">
         <is>
           <t>Sometimes</t>
@@ -69754,6 +70839,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K1073" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L1073" t="inlineStr">
         <is>
           <t>Always</t>
@@ -69892,6 +70982,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K1075" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L1075" t="inlineStr">
         <is>
           <t>Often</t>
@@ -69960,6 +71055,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K1076" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L1076" t="inlineStr">
         <is>
           <t>Sometimes</t>
@@ -70131,6 +71231,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K1080" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L1080" t="inlineStr">
         <is>
           <t>Sometimes</t>
@@ -70272,6 +71377,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K1082" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L1082" t="inlineStr">
         <is>
           <t>Sometimes</t>
@@ -70408,6 +71518,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K1084" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L1084" t="inlineStr">
         <is>
           <t>Decline to answer</t>
@@ -70705,6 +71820,11 @@
           <t>Not in Poverty</t>
         </is>
       </c>
+      <c r="K1089" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L1089" t="inlineStr">
         <is>
           <t>Never</t>
@@ -70841,6 +71961,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K1091" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L1091" t="inlineStr">
         <is>
           <t>Always</t>
@@ -71201,6 +72326,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K1098" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L1098" t="inlineStr">
         <is>
           <t>Never</t>
@@ -71669,6 +72799,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K1107" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L1107" t="inlineStr">
         <is>
           <t>Never</t>
@@ -72610,6 +73745,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K1121" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L1121" t="inlineStr">
         <is>
           <t>Sometimes</t>
@@ -72751,6 +73891,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K1123" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L1123" t="inlineStr">
         <is>
           <t>Often</t>
@@ -72819,6 +73964,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K1124" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L1124" t="inlineStr">
         <is>
           <t>Always</t>
@@ -73101,6 +74251,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K1128" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L1128" t="inlineStr">
         <is>
           <t>Never</t>
@@ -73232,6 +74387,11 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="K1130" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L1130" t="inlineStr">
         <is>
           <t>Never</t>
@@ -73300,6 +74460,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K1131" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L1131" t="inlineStr">
         <is>
           <t>Sometimes</t>
@@ -73594,6 +74759,11 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="K1136" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L1136" t="inlineStr">
         <is>
           <t>Always</t>
@@ -73918,6 +75088,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K1144" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L1144" t="inlineStr">
         <is>
           <t>Never</t>
@@ -73978,6 +75153,11 @@
           <t>Not in Poverty</t>
         </is>
       </c>
+      <c r="K1145" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L1145" t="inlineStr">
         <is>
           <t>Always</t>
@@ -74265,6 +75445,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K1149" t="inlineStr">
+        <is>
+          <t>In labor force</t>
+        </is>
+      </c>
       <c r="L1149" t="inlineStr">
         <is>
           <t>Always</t>
@@ -74627,6 +75812,11 @@
       <c r="J1155" t="inlineStr">
         <is>
           <t>No</t>
+        </is>
+      </c>
+      <c r="K1155" t="inlineStr">
+        <is>
+          <t>In labor force</t>
         </is>
       </c>
       <c r="L1155" t="inlineStr">

</xml_diff>